<commit_message>
feat: month and week algorithm
</commit_message>
<xml_diff>
--- a/excel/List Tugas Gabunggan.xlsx
+++ b/excel/List Tugas Gabunggan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\File Tugas Sekolah\System Support\Tugas\Semester 2\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\Programs\Web Dev Related Stuff\Web Dev\Web Laporan V.5\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F3E6BE-0835-41BC-BE97-4589EC410657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD6FC9E-6C05-4264-824A-F5DB10EFADE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$K$39</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="104">
   <si>
     <t>No.</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>PKK8</t>
+  </si>
+  <si>
+    <t>Bulan Ke-1</t>
+  </si>
+  <si>
+    <t>Bulan Ke-2</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -563,18 +569,6 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -587,7 +581,22 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -896,13 +905,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT45"/>
+  <dimension ref="A1:AT39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AV7" sqref="AV7"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AN5" sqref="AN5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,8 +931,7 @@
     <col min="19" max="19" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.109375" style="1" customWidth="1"/>
+    <col min="22" max="24" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="34" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -945,411 +953,407 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+    </row>
+    <row r="2" spans="1:46" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="28" t="s">
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="29" t="s">
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="27" t="s">
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="30" t="s">
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="28" t="s">
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="29" t="s">
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="30"/>
+      <c r="AL2" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="27" t="s">
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="30" t="s">
+      <c r="AP2" s="27"/>
+      <c r="AQ2" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-    </row>
-    <row r="2" spans="1:46" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="25" t="s">
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="29"/>
+      <c r="AT2" s="29"/>
+    </row>
+    <row r="3" spans="1:46" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E3" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H3" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I3" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J3" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K3" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L3" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="O3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P3" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="23" t="s">
+      <c r="Q3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="26" t="s">
+      <c r="S3" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="26" t="s">
+      <c r="T3" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="U3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="V3" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="25" t="s">
+      <c r="W3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="25" t="s">
+      <c r="X3" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" s="25" t="s">
+      <c r="Y3" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" s="24" t="s">
+      <c r="Z3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="24" t="s">
+      <c r="AA3" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="24" t="s">
+      <c r="AB3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="AC2" s="24" t="s">
+      <c r="AC3" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AD2" s="24" t="s">
+      <c r="AD3" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AE2" s="24" t="s">
+      <c r="AE3" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="AF2" s="23" t="s">
+      <c r="AF3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="AG2" s="23" t="s">
+      <c r="AG3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AH2" s="23" t="s">
+      <c r="AH3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AI2" s="23" t="s">
+      <c r="AI3" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AJ2" s="23" t="s">
+      <c r="AJ3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="AK2" s="23" t="s">
+      <c r="AK3" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="AL2" s="26" t="s">
+      <c r="AL3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="AM2" s="26" t="s">
+      <c r="AM3" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AN2" s="26" t="s">
+      <c r="AN3" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="AO2" s="25" t="s">
+      <c r="AO3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AP2" s="25" t="s">
+      <c r="AP3" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AQ2" s="24" t="s">
+      <c r="AQ3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AR2" s="24" t="s">
+      <c r="AR3" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="AS2" s="24" t="s">
+      <c r="AS3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="AT2" s="24" t="s">
+      <c r="AT3" s="26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="2" t="s">
+    <row r="4" spans="1:46" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M4" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N4" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O4" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P4" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q4" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R4" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="S4" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="T4" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="U4" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="V4" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Y4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="Z4" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AA4" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AB4" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AC4" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AD4" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AE4" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AF3" s="14" t="s">
+      <c r="AF4" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="AG3" s="14" t="s">
+      <c r="AG4" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="AH3" s="14" t="s">
+      <c r="AH4" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="AI3" s="14" t="s">
+      <c r="AI4" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AJ3" s="14" t="s">
+      <c r="AJ4" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AK3" s="14" t="s">
+      <c r="AK4" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="AL3" s="17" t="s">
+      <c r="AL4" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="AM3" s="17" t="s">
+      <c r="AM4" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AN3" s="17" t="s">
+      <c r="AN4" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="AO3" s="2" t="s">
+      <c r="AO4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="AP3" s="2" t="s">
+      <c r="AP4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AQ3" s="6" t="s">
+      <c r="AQ4" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AR3" s="6" t="s">
+      <c r="AR4" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="AS3" s="6" t="s">
+      <c r="AS4" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="AT3" s="6" t="s">
+      <c r="AT4" s="6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="13"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="13"/>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="13"/>
-      <c r="AL4" s="15"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="15"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="18"/>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="8"/>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="8"/>
     </row>
     <row r="5" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>40</v>
@@ -1402,12 +1406,14 @@
     </row>
     <row r="6" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
@@ -1449,19 +1455,17 @@
       <c r="AN6" s="15"/>
       <c r="AO6" s="4"/>
       <c r="AP6" s="18"/>
-      <c r="AQ6" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="AQ6" s="7"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="7"/>
       <c r="AT6" s="8"/>
     </row>
     <row r="7" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="8"/>
@@ -1505,21 +1509,21 @@
       <c r="AN7" s="15"/>
       <c r="AO7" s="4"/>
       <c r="AP7" s="18"/>
-      <c r="AQ7" s="7"/>
+      <c r="AQ7" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="AR7" s="8"/>
       <c r="AS7" s="7"/>
       <c r="AT7" s="8"/>
     </row>
     <row r="8" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="8"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
@@ -1553,9 +1557,7 @@
       <c r="AF8" s="12"/>
       <c r="AG8" s="13"/>
       <c r="AH8" s="12"/>
-      <c r="AI8" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="AI8" s="13"/>
       <c r="AJ8" s="12"/>
       <c r="AK8" s="13"/>
       <c r="AL8" s="15"/>
@@ -1564,24 +1566,20 @@
       <c r="AO8" s="4"/>
       <c r="AP8" s="18"/>
       <c r="AQ8" s="7"/>
-      <c r="AR8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT8" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="AR8" s="8"/>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="8"/>
     </row>
     <row r="9" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
@@ -1615,7 +1613,9 @@
       <c r="AF9" s="12"/>
       <c r="AG9" s="13"/>
       <c r="AH9" s="12"/>
-      <c r="AI9" s="13"/>
+      <c r="AI9" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="AJ9" s="12"/>
       <c r="AK9" s="13"/>
       <c r="AL9" s="15"/>
@@ -1624,20 +1624,24 @@
       <c r="AO9" s="4"/>
       <c r="AP9" s="18"/>
       <c r="AQ9" s="7"/>
-      <c r="AR9" s="8"/>
-      <c r="AS9" s="7"/>
-      <c r="AT9" s="8"/>
+      <c r="AR9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT9" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="8"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
@@ -1686,12 +1690,14 @@
     </row>
     <row r="11" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
@@ -1740,14 +1746,12 @@
     </row>
     <row r="12" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="8"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
@@ -1781,9 +1785,7 @@
       <c r="AF12" s="12"/>
       <c r="AG12" s="13"/>
       <c r="AH12" s="12"/>
-      <c r="AI12" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="AI12" s="13"/>
       <c r="AJ12" s="12"/>
       <c r="AK12" s="13"/>
       <c r="AL12" s="15"/>
@@ -1791,27 +1793,21 @@
       <c r="AN12" s="15"/>
       <c r="AO12" s="4"/>
       <c r="AP12" s="18"/>
-      <c r="AQ12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT12" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="AQ12" s="7"/>
+      <c r="AR12" s="8"/>
+      <c r="AS12" s="7"/>
+      <c r="AT12" s="8"/>
     </row>
     <row r="13" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
@@ -1845,7 +1841,9 @@
       <c r="AF13" s="12"/>
       <c r="AG13" s="13"/>
       <c r="AH13" s="12"/>
-      <c r="AI13" s="13"/>
+      <c r="AI13" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="AJ13" s="12"/>
       <c r="AK13" s="13"/>
       <c r="AL13" s="15"/>
@@ -1853,17 +1851,25 @@
       <c r="AN13" s="15"/>
       <c r="AO13" s="4"/>
       <c r="AP13" s="18"/>
-      <c r="AQ13" s="7"/>
-      <c r="AR13" s="8"/>
-      <c r="AS13" s="7"/>
-      <c r="AT13" s="8"/>
+      <c r="AQ13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR13" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT13" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="8"/>
@@ -1914,23 +1920,19 @@
     </row>
     <row r="15" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C15" s="4"/>
       <c r="D15" s="8"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="J15" s="8"/>
       <c r="K15" s="9" t="s">
         <v>40</v>
       </c>
@@ -1943,9 +1945,7 @@
       <c r="R15" s="15"/>
       <c r="S15" s="16"/>
       <c r="T15" s="15"/>
-      <c r="U15" s="16" t="s">
-        <v>59</v>
-      </c>
+      <c r="U15" s="16"/>
       <c r="V15" s="15"/>
       <c r="W15" s="4"/>
       <c r="X15" s="18"/>
@@ -1963,42 +1963,34 @@
       <c r="AJ15" s="12"/>
       <c r="AK15" s="13"/>
       <c r="AL15" s="15"/>
-      <c r="AM15" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN15" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP15" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ15" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="AM15" s="16"/>
+      <c r="AN15" s="15"/>
+      <c r="AO15" s="4"/>
+      <c r="AP15" s="18"/>
+      <c r="AQ15" s="7"/>
       <c r="AR15" s="8"/>
       <c r="AS15" s="7"/>
-      <c r="AT15" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="AT15" s="8"/>
     </row>
     <row r="16" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
+      <c r="J16" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="K16" s="9" t="s">
         <v>40</v>
       </c>
@@ -2011,7 +2003,9 @@
       <c r="R16" s="15"/>
       <c r="S16" s="16"/>
       <c r="T16" s="15"/>
-      <c r="U16" s="16"/>
+      <c r="U16" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="V16" s="15"/>
       <c r="W16" s="4"/>
       <c r="X16" s="18"/>
@@ -2029,21 +2023,33 @@
       <c r="AJ16" s="12"/>
       <c r="AK16" s="13"/>
       <c r="AL16" s="15"/>
-      <c r="AM16" s="16"/>
-      <c r="AN16" s="15"/>
-      <c r="AO16" s="4"/>
-      <c r="AP16" s="18"/>
-      <c r="AQ16" s="7"/>
+      <c r="AM16" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP16" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ16" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="AR16" s="8"/>
       <c r="AS16" s="7"/>
-      <c r="AT16" s="8"/>
+      <c r="AT16" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="8"/>
@@ -2094,10 +2100,10 @@
     </row>
     <row r="18" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="8"/>
@@ -2148,10 +2154,10 @@
     </row>
     <row r="19" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="8"/>
@@ -2202,10 +2208,10 @@
     </row>
     <row r="20" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="8"/>
@@ -2249,25 +2255,17 @@
       <c r="AN20" s="15"/>
       <c r="AO20" s="4"/>
       <c r="AP20" s="18"/>
-      <c r="AQ20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR20" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT20" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="AQ20" s="7"/>
+      <c r="AR20" s="8"/>
+      <c r="AS20" s="7"/>
+      <c r="AT20" s="8"/>
     </row>
     <row r="21" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="8"/>
@@ -2311,21 +2309,27 @@
       <c r="AN21" s="15"/>
       <c r="AO21" s="4"/>
       <c r="AP21" s="18"/>
-      <c r="AQ21" s="7"/>
-      <c r="AR21" s="8"/>
-      <c r="AS21" s="7"/>
-      <c r="AT21" s="8"/>
+      <c r="AQ21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT21" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C22" s="4"/>
       <c r="D22" s="8"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
@@ -2374,12 +2378,14 @@
     </row>
     <row r="23" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D23" s="8"/>
       <c r="E23" s="7"/>
       <c r="F23" s="8"/>
@@ -2428,10 +2434,10 @@
     </row>
     <row r="24" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="8"/>
@@ -2482,10 +2488,10 @@
     </row>
     <row r="25" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="8"/>
@@ -2529,23 +2535,19 @@
       <c r="AN25" s="15"/>
       <c r="AO25" s="4"/>
       <c r="AP25" s="18"/>
-      <c r="AQ25" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="AQ25" s="7"/>
       <c r="AR25" s="8"/>
       <c r="AS25" s="7"/>
       <c r="AT25" s="8"/>
     </row>
     <row r="26" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="8"/>
       <c r="E26" s="7"/>
       <c r="F26" s="8"/>
@@ -2579,9 +2581,7 @@
       <c r="AF26" s="12"/>
       <c r="AG26" s="13"/>
       <c r="AH26" s="12"/>
-      <c r="AI26" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="AI26" s="13"/>
       <c r="AJ26" s="12"/>
       <c r="AK26" s="13"/>
       <c r="AL26" s="15"/>
@@ -2592,33 +2592,27 @@
       <c r="AQ26" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AR26" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT26" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="AR26" s="8"/>
+      <c r="AS26" s="7"/>
+      <c r="AT26" s="8"/>
     </row>
     <row r="27" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D27" s="8"/>
       <c r="E27" s="7"/>
       <c r="F27" s="8"/>
       <c r="G27" s="7"/>
       <c r="H27" s="8"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="J27" s="8"/>
       <c r="K27" s="9" t="s">
         <v>40</v>
       </c>
@@ -2631,9 +2625,7 @@
       <c r="R27" s="15"/>
       <c r="S27" s="16"/>
       <c r="T27" s="15"/>
-      <c r="U27" s="16" t="s">
-        <v>59</v>
-      </c>
+      <c r="U27" s="16"/>
       <c r="V27" s="15"/>
       <c r="W27" s="4"/>
       <c r="X27" s="18"/>
@@ -2647,38 +2639,46 @@
       <c r="AF27" s="12"/>
       <c r="AG27" s="13"/>
       <c r="AH27" s="12"/>
-      <c r="AI27" s="13"/>
+      <c r="AI27" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="AJ27" s="12"/>
       <c r="AK27" s="13"/>
       <c r="AL27" s="15"/>
       <c r="AM27" s="16"/>
-      <c r="AN27" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="AN27" s="15"/>
       <c r="AO27" s="4"/>
       <c r="AP27" s="18"/>
-      <c r="AQ27" s="7"/>
-      <c r="AR27" s="8"/>
-      <c r="AS27" s="7"/>
-      <c r="AT27" s="8"/>
+      <c r="AQ27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR27" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT27" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="8"/>
       <c r="E28" s="7"/>
       <c r="F28" s="8"/>
       <c r="G28" s="7"/>
       <c r="H28" s="8"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="8"/>
+      <c r="J28" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="K28" s="9" t="s">
         <v>40</v>
       </c>
@@ -2691,7 +2691,9 @@
       <c r="R28" s="15"/>
       <c r="S28" s="16"/>
       <c r="T28" s="15"/>
-      <c r="U28" s="16"/>
+      <c r="U28" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="V28" s="15"/>
       <c r="W28" s="4"/>
       <c r="X28" s="18"/>
@@ -2710,7 +2712,9 @@
       <c r="AK28" s="13"/>
       <c r="AL28" s="15"/>
       <c r="AM28" s="16"/>
-      <c r="AN28" s="15"/>
+      <c r="AN28" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="AO28" s="4"/>
       <c r="AP28" s="18"/>
       <c r="AQ28" s="7"/>
@@ -2720,21 +2724,21 @@
     </row>
     <row r="29" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D29" s="8"/>
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
       <c r="G29" s="7"/>
       <c r="H29" s="8"/>
       <c r="I29" s="7"/>
-      <c r="J29" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="J29" s="8"/>
       <c r="K29" s="9" t="s">
         <v>40</v>
       </c>
@@ -2747,9 +2751,7 @@
       <c r="R29" s="15"/>
       <c r="S29" s="16"/>
       <c r="T29" s="15"/>
-      <c r="U29" s="16" t="s">
-        <v>59</v>
-      </c>
+      <c r="U29" s="16"/>
       <c r="V29" s="15"/>
       <c r="W29" s="4"/>
       <c r="X29" s="18"/>
@@ -2768,9 +2770,7 @@
       <c r="AK29" s="13"/>
       <c r="AL29" s="15"/>
       <c r="AM29" s="16"/>
-      <c r="AN29" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="AN29" s="15"/>
       <c r="AO29" s="4"/>
       <c r="AP29" s="18"/>
       <c r="AQ29" s="7"/>
@@ -2780,10 +2780,10 @@
     </row>
     <row r="30" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="8"/>
@@ -2792,7 +2792,9 @@
       <c r="G30" s="7"/>
       <c r="H30" s="8"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="8"/>
+      <c r="J30" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="K30" s="9" t="s">
         <v>40</v>
       </c>
@@ -2805,7 +2807,9 @@
       <c r="R30" s="15"/>
       <c r="S30" s="16"/>
       <c r="T30" s="15"/>
-      <c r="U30" s="16"/>
+      <c r="U30" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="V30" s="15"/>
       <c r="W30" s="4"/>
       <c r="X30" s="18"/>
@@ -2824,7 +2828,9 @@
       <c r="AK30" s="13"/>
       <c r="AL30" s="15"/>
       <c r="AM30" s="16"/>
-      <c r="AN30" s="15"/>
+      <c r="AN30" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="AO30" s="4"/>
       <c r="AP30" s="18"/>
       <c r="AQ30" s="7"/>
@@ -2834,14 +2840,12 @@
     </row>
     <row r="31" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C31" s="4"/>
       <c r="D31" s="8"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -2890,21 +2894,21 @@
     </row>
     <row r="32" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="9"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="10"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="8"/>
       <c r="K32" s="9" t="s">
         <v>40</v>
       </c>
@@ -2922,18 +2926,16 @@
       <c r="W32" s="4"/>
       <c r="X32" s="18"/>
       <c r="Y32" s="19"/>
-      <c r="Z32" s="10"/>
-      <c r="AA32" s="9"/>
-      <c r="AB32" s="10"/>
-      <c r="AC32" s="9"/>
-      <c r="AD32" s="10"/>
-      <c r="AE32" s="9"/>
+      <c r="Z32" s="8"/>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="8"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="8"/>
+      <c r="AE32" s="7"/>
       <c r="AF32" s="12"/>
       <c r="AG32" s="13"/>
       <c r="AH32" s="12"/>
-      <c r="AI32" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="AI32" s="13"/>
       <c r="AJ32" s="12"/>
       <c r="AK32" s="13"/>
       <c r="AL32" s="15"/>
@@ -2941,34 +2943,28 @@
       <c r="AN32" s="15"/>
       <c r="AO32" s="4"/>
       <c r="AP32" s="18"/>
-      <c r="AQ32" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR32" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS32" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT32" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="AQ32" s="7"/>
+      <c r="AR32" s="8"/>
+      <c r="AS32" s="7"/>
+      <c r="AT32" s="8"/>
     </row>
     <row r="33" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="9"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="8"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="10"/>
       <c r="K33" s="9" t="s">
         <v>40</v>
       </c>
@@ -2986,16 +2982,18 @@
       <c r="W33" s="4"/>
       <c r="X33" s="18"/>
       <c r="Y33" s="19"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="8"/>
-      <c r="AC33" s="7"/>
-      <c r="AD33" s="8"/>
-      <c r="AE33" s="7"/>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="9"/>
+      <c r="AB33" s="10"/>
+      <c r="AC33" s="9"/>
+      <c r="AD33" s="10"/>
+      <c r="AE33" s="9"/>
       <c r="AF33" s="12"/>
       <c r="AG33" s="13"/>
       <c r="AH33" s="12"/>
-      <c r="AI33" s="13"/>
+      <c r="AI33" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="AJ33" s="12"/>
       <c r="AK33" s="13"/>
       <c r="AL33" s="15"/>
@@ -3003,17 +3001,25 @@
       <c r="AN33" s="15"/>
       <c r="AO33" s="4"/>
       <c r="AP33" s="18"/>
-      <c r="AQ33" s="7"/>
-      <c r="AR33" s="8"/>
-      <c r="AS33" s="7"/>
-      <c r="AT33" s="8"/>
+      <c r="AQ33" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR33" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS33" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT33" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="34" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="8"/>
@@ -3057,27 +3063,19 @@
       <c r="AN34" s="15"/>
       <c r="AO34" s="4"/>
       <c r="AP34" s="18"/>
-      <c r="AQ34" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR34" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS34" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="AQ34" s="7"/>
+      <c r="AR34" s="8"/>
+      <c r="AS34" s="7"/>
       <c r="AT34" s="8"/>
     </row>
     <row r="35" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C35" s="4"/>
       <c r="D35" s="8"/>
       <c r="E35" s="7"/>
       <c r="F35" s="8"/>
@@ -3119,17 +3117,23 @@
       <c r="AN35" s="15"/>
       <c r="AO35" s="4"/>
       <c r="AP35" s="18"/>
-      <c r="AQ35" s="7"/>
-      <c r="AR35" s="8"/>
-      <c r="AS35" s="7"/>
+      <c r="AQ35" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR35" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS35" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="AT35" s="8"/>
     </row>
     <row r="36" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>40</v>
@@ -3182,10 +3186,10 @@
     </row>
     <row r="37" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>40</v>
@@ -3238,21 +3242,21 @@
     </row>
     <row r="38" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D38" s="8"/>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
       <c r="G38" s="7"/>
       <c r="H38" s="8"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="J38" s="8"/>
       <c r="K38" s="9" t="s">
         <v>40</v>
       </c>
@@ -3265,9 +3269,7 @@
       <c r="R38" s="15"/>
       <c r="S38" s="16"/>
       <c r="T38" s="15"/>
-      <c r="U38" s="16" t="s">
-        <v>59</v>
-      </c>
+      <c r="U38" s="16"/>
       <c r="V38" s="15"/>
       <c r="W38" s="4"/>
       <c r="X38" s="18"/>
@@ -3286,9 +3288,7 @@
       <c r="AK38" s="13"/>
       <c r="AL38" s="15"/>
       <c r="AM38" s="16"/>
-      <c r="AN38" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="AN38" s="15"/>
       <c r="AO38" s="4"/>
       <c r="AP38" s="18"/>
       <c r="AQ38" s="7"/>
@@ -3296,30 +3296,86 @@
       <c r="AS38" s="7"/>
       <c r="AT38" s="8"/>
     </row>
-    <row r="40" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:46" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:46" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:46" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
+        <v>35</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L39" s="8"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="V39" s="15"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="18"/>
+      <c r="Y39" s="19"/>
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="8"/>
+      <c r="AC39" s="7"/>
+      <c r="AD39" s="8"/>
+      <c r="AE39" s="7"/>
+      <c r="AF39" s="12"/>
+      <c r="AG39" s="13"/>
+      <c r="AH39" s="12"/>
+      <c r="AI39" s="13"/>
+      <c r="AJ39" s="12"/>
+      <c r="AK39" s="13"/>
+      <c r="AL39" s="15"/>
+      <c r="AM39" s="16"/>
+      <c r="AN39" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO39" s="4"/>
+      <c r="AP39" s="18"/>
+      <c r="AQ39" s="7"/>
+      <c r="AR39" s="8"/>
+      <c r="AS39" s="7"/>
+      <c r="AT39" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="D1:L1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AF1:AK1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="Z1:AE1"/>
-    <mergeCell ref="AQ1:AT1"/>
+  <mergeCells count="13">
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="C1:V1"/>
+    <mergeCell ref="W1:AT1"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AE2"/>
+    <mergeCell ref="AF2:AK2"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="M2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B4:B38">
+  <conditionalFormatting sqref="B5:B39">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text=",">
-      <formula>NOT(ISERROR(SEARCH(",",B4)))</formula>
+      <formula>NOT(ISERROR(SEARCH(",",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>